<commit_message>
Ya puedo usar los ints del excel
Era un problema con el origen del for, al parecer. Ahora sigue procesar
todo el archivo
</commit_message>
<xml_diff>
--- a/Borradores/Parametrizacion/Estructura de las matrices.xlsx
+++ b/Borradores/Parametrizacion/Estructura de las matrices.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="92">
   <si>
     <t>Nombre de la matriz</t>
   </si>
@@ -235,6 +235,63 @@
   </si>
   <si>
     <t>Float</t>
+  </si>
+  <si>
+    <t>Mes</t>
+  </si>
+  <si>
+    <t>Fecha de diligenciamiento Desde</t>
+  </si>
+  <si>
+    <t>Fecha de diligenciamiento Desde Mes</t>
+  </si>
+  <si>
+    <t>Día</t>
+  </si>
+  <si>
+    <t>Fecha de diligenciamiento Hasta</t>
+  </si>
+  <si>
+    <t>Profesional responsable</t>
+  </si>
+  <si>
+    <t>Año</t>
+  </si>
+  <si>
+    <t>Descripción general del proceso de captura de información</t>
+  </si>
+  <si>
+    <t>Departamento</t>
+  </si>
+  <si>
+    <t>Número de alcaldes</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>Sector Representado</t>
+  </si>
+  <si>
+    <t>Nombre del consejero</t>
+  </si>
+  <si>
+    <t>Entidad / Empresa / Gremio</t>
+  </si>
+  <si>
+    <t>Nombre del director general de CAR</t>
+  </si>
+  <si>
+    <t>Fecha de posesión del actual director Día</t>
+  </si>
+  <si>
+    <t>Fecha de posesión del actual director Mes</t>
+  </si>
+  <si>
+    <t>Fecha de posesión del actual director Año</t>
+  </si>
+  <si>
+    <t>Diá</t>
   </si>
 </sst>
 </file>
@@ -1560,8 +1617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K202"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="C70" workbookViewId="0">
+      <selection activeCell="K90" sqref="K90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1635,7 +1692,7 @@
         <v>5</v>
       </c>
       <c r="J3">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K3" t="s">
         <v>58</v>
@@ -1670,7 +1727,7 @@
         <v>4</v>
       </c>
       <c r="J4">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K4" t="s">
         <v>58</v>
@@ -1705,7 +1762,7 @@
         <v>4</v>
       </c>
       <c r="J5">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K5" t="s">
         <v>58</v>
@@ -1740,7 +1797,7 @@
         <v>4</v>
       </c>
       <c r="J6">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K6" t="s">
         <v>58</v>
@@ -1772,7 +1829,7 @@
         <v>4</v>
       </c>
       <c r="J7">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K7" t="s">
         <v>58</v>
@@ -1807,7 +1864,7 @@
         <v>4</v>
       </c>
       <c r="J8">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K8" t="s">
         <v>58</v>
@@ -1839,7 +1896,7 @@
         <v>5</v>
       </c>
       <c r="J9">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K9" t="s">
         <v>58</v>
@@ -1871,7 +1928,7 @@
         <v>8</v>
       </c>
       <c r="J10">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K10" t="s">
         <v>58</v>
@@ -1906,7 +1963,7 @@
         <v>5</v>
       </c>
       <c r="J11">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K11" t="s">
         <v>58</v>
@@ -1941,7 +1998,7 @@
         <v>8</v>
       </c>
       <c r="J12">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K12" t="s">
         <v>58</v>
@@ -1976,7 +2033,7 @@
         <v>5</v>
       </c>
       <c r="J13">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K13" t="s">
         <v>58</v>
@@ -2011,7 +2068,7 @@
         <v>6</v>
       </c>
       <c r="J14">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K14" t="s">
         <v>58</v>
@@ -2046,7 +2103,7 @@
         <v>4</v>
       </c>
       <c r="J15">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K15" t="s">
         <v>58</v>
@@ -2081,7 +2138,7 @@
         <v>4</v>
       </c>
       <c r="J16">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K16" t="s">
         <v>58</v>
@@ -2116,7 +2173,7 @@
         <v>4</v>
       </c>
       <c r="J17">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K17" t="s">
         <v>58</v>
@@ -2148,7 +2205,7 @@
         <v>4</v>
       </c>
       <c r="J18">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K18" t="s">
         <v>58</v>
@@ -2158,388 +2215,2413 @@
       <c r="A19">
         <v>17</v>
       </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19">
+        <v>4</v>
+      </c>
+      <c r="G19">
+        <v>41</v>
+      </c>
+      <c r="I19">
+        <v>4</v>
+      </c>
+      <c r="J19">
+        <v>42</v>
+      </c>
+      <c r="K19" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" t="s">
+        <v>76</v>
+      </c>
+      <c r="F20">
+        <v>5</v>
+      </c>
+      <c r="G20">
+        <v>41</v>
+      </c>
+      <c r="I20">
+        <v>5</v>
+      </c>
+      <c r="J20">
+        <v>42</v>
+      </c>
+      <c r="K20" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E21" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21">
+        <v>6</v>
+      </c>
+      <c r="G21">
+        <v>41</v>
+      </c>
+      <c r="I21">
+        <v>6</v>
+      </c>
+      <c r="J21">
+        <v>42</v>
+      </c>
+      <c r="K21" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22">
+        <v>4</v>
+      </c>
+      <c r="G22">
+        <v>41</v>
+      </c>
+      <c r="I22">
+        <v>4</v>
+      </c>
+      <c r="J22">
+        <v>43</v>
+      </c>
+      <c r="K22" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>77</v>
+      </c>
+      <c r="E23" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23">
+        <v>5</v>
+      </c>
+      <c r="G23">
+        <v>41</v>
+      </c>
+      <c r="I23">
+        <v>5</v>
+      </c>
+      <c r="J23">
+        <v>43</v>
+      </c>
+      <c r="K23" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24">
+        <v>6</v>
+      </c>
+      <c r="G24">
+        <v>41</v>
+      </c>
+      <c r="I24">
+        <v>6</v>
+      </c>
+      <c r="J24">
+        <v>43</v>
+      </c>
+      <c r="K24" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" t="s">
+        <v>78</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>45</v>
+      </c>
+      <c r="I25">
+        <v>3</v>
+      </c>
+      <c r="J25">
+        <v>45</v>
+      </c>
+      <c r="K25" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" t="s">
+        <v>80</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>48</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>49</v>
+      </c>
+      <c r="K26" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>81</v>
+      </c>
+      <c r="E27" t="s">
+        <v>81</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>11</v>
+      </c>
+      <c r="I27">
+        <v>3</v>
+      </c>
+      <c r="J27">
+        <v>11</v>
+      </c>
+      <c r="K27" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28" t="s">
+        <v>82</v>
+      </c>
+      <c r="F28">
+        <v>5</v>
+      </c>
+      <c r="G28">
+        <v>11</v>
+      </c>
+      <c r="I28">
+        <v>7</v>
+      </c>
+      <c r="J28">
+        <v>11</v>
+      </c>
+      <c r="K28" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>81</v>
+      </c>
+      <c r="E29" t="s">
+        <v>81</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>12</v>
+      </c>
+      <c r="I29">
+        <v>3</v>
+      </c>
+      <c r="J29">
+        <v>12</v>
+      </c>
+      <c r="K29" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30" t="s">
+        <v>82</v>
+      </c>
+      <c r="E30" t="s">
+        <v>82</v>
+      </c>
+      <c r="F30">
+        <v>5</v>
+      </c>
+      <c r="G30">
+        <v>12</v>
+      </c>
+      <c r="I30">
+        <v>7</v>
+      </c>
+      <c r="J30">
+        <v>12</v>
+      </c>
+      <c r="K30" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31" t="s">
+        <v>81</v>
+      </c>
+      <c r="E31" t="s">
+        <v>81</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>13</v>
+      </c>
+      <c r="I31">
+        <v>3</v>
+      </c>
+      <c r="J31">
+        <v>13</v>
+      </c>
+      <c r="K31" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32" t="s">
+        <v>82</v>
+      </c>
+      <c r="E32" t="s">
+        <v>82</v>
+      </c>
+      <c r="F32">
+        <v>5</v>
+      </c>
+      <c r="G32">
+        <v>13</v>
+      </c>
+      <c r="I32">
+        <v>7</v>
+      </c>
+      <c r="J32">
+        <v>13</v>
+      </c>
+      <c r="K32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33" t="s">
+        <v>81</v>
+      </c>
+      <c r="E33" t="s">
+        <v>81</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>14</v>
+      </c>
+      <c r="I33">
+        <v>3</v>
+      </c>
+      <c r="J33">
+        <v>14</v>
+      </c>
+      <c r="K33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34" t="s">
+        <v>82</v>
+      </c>
+      <c r="E34" t="s">
+        <v>82</v>
+      </c>
+      <c r="F34">
+        <v>5</v>
+      </c>
+      <c r="G34">
+        <v>14</v>
+      </c>
+      <c r="I34">
+        <v>7</v>
+      </c>
+      <c r="J34">
+        <v>14</v>
+      </c>
+      <c r="K34" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35" t="s">
+        <v>81</v>
+      </c>
+      <c r="E35" t="s">
+        <v>81</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>15</v>
+      </c>
+      <c r="I35">
+        <v>3</v>
+      </c>
+      <c r="J35">
+        <v>15</v>
+      </c>
+      <c r="K35" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36" t="s">
+        <v>82</v>
+      </c>
+      <c r="E36" t="s">
+        <v>82</v>
+      </c>
+      <c r="F36">
+        <v>5</v>
+      </c>
+      <c r="G36">
+        <v>15</v>
+      </c>
+      <c r="I36">
+        <v>7</v>
+      </c>
+      <c r="J36">
+        <v>15</v>
+      </c>
+      <c r="K36" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37" t="s">
+        <v>81</v>
+      </c>
+      <c r="E37" t="s">
+        <v>81</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>16</v>
+      </c>
+      <c r="I37">
+        <v>3</v>
+      </c>
+      <c r="J37">
+        <v>16</v>
+      </c>
+      <c r="K37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>3</v>
+      </c>
+      <c r="D38" t="s">
+        <v>82</v>
+      </c>
+      <c r="E38" t="s">
+        <v>82</v>
+      </c>
+      <c r="F38">
+        <v>5</v>
+      </c>
+      <c r="G38">
+        <v>16</v>
+      </c>
+      <c r="I38">
+        <v>7</v>
+      </c>
+      <c r="J38">
+        <v>16</v>
+      </c>
+      <c r="K38" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39" t="s">
+        <v>84</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>21</v>
+      </c>
+      <c r="I39">
+        <v>2</v>
+      </c>
+      <c r="J39">
+        <v>21</v>
+      </c>
+      <c r="K39" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="D40" t="s">
+        <v>85</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>21</v>
+      </c>
+      <c r="I40">
+        <v>4</v>
+      </c>
+      <c r="J40">
+        <v>21</v>
+      </c>
+      <c r="K40" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41" t="s">
+        <v>86</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>21</v>
+      </c>
+      <c r="I41">
+        <v>6</v>
+      </c>
+      <c r="J41">
+        <v>21</v>
+      </c>
+      <c r="K41" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="D42" t="s">
+        <v>84</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>22</v>
+      </c>
+      <c r="I42">
+        <v>2</v>
+      </c>
+      <c r="J42">
+        <v>22</v>
+      </c>
+      <c r="K42" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>3</v>
+      </c>
+      <c r="D43" t="s">
+        <v>85</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <v>22</v>
+      </c>
+      <c r="I43">
+        <v>4</v>
+      </c>
+      <c r="J43">
+        <v>22</v>
+      </c>
+      <c r="K43" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44" t="s">
+        <v>86</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <v>22</v>
+      </c>
+      <c r="I44">
+        <v>6</v>
+      </c>
+      <c r="J44">
+        <v>22</v>
+      </c>
+      <c r="K44" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45" t="s">
+        <v>84</v>
+      </c>
+      <c r="E45">
+        <v>3</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="G45">
+        <v>23</v>
+      </c>
+      <c r="I45">
+        <v>2</v>
+      </c>
+      <c r="J45">
+        <v>23</v>
+      </c>
+      <c r="K45" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46" t="s">
+        <v>85</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46">
+        <v>23</v>
+      </c>
+      <c r="I46">
+        <v>4</v>
+      </c>
+      <c r="J46">
+        <v>23</v>
+      </c>
+      <c r="K46" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="D47" t="s">
+        <v>86</v>
+      </c>
+      <c r="E47">
+        <v>3</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+      <c r="G47">
+        <v>23</v>
+      </c>
+      <c r="I47">
+        <v>6</v>
+      </c>
+      <c r="J47">
+        <v>23</v>
+      </c>
+      <c r="K47" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>3</v>
+      </c>
+      <c r="D48" t="s">
+        <v>84</v>
+      </c>
+      <c r="E48">
+        <v>4</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+      <c r="G48">
+        <v>24</v>
+      </c>
+      <c r="I48">
+        <v>2</v>
+      </c>
+      <c r="J48">
+        <v>24</v>
+      </c>
+      <c r="K48" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49" t="s">
+        <v>85</v>
+      </c>
+      <c r="E49">
+        <v>4</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="G49">
+        <v>24</v>
+      </c>
+      <c r="I49">
+        <v>4</v>
+      </c>
+      <c r="J49">
+        <v>24</v>
+      </c>
+      <c r="K49" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>3</v>
+      </c>
+      <c r="D50" t="s">
+        <v>86</v>
+      </c>
+      <c r="E50">
+        <v>4</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <v>24</v>
+      </c>
+      <c r="I50">
+        <v>6</v>
+      </c>
+      <c r="J50">
+        <v>24</v>
+      </c>
+      <c r="K50" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>3</v>
+      </c>
+      <c r="D51" t="s">
+        <v>84</v>
+      </c>
+      <c r="E51">
+        <v>5</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51">
+        <v>25</v>
+      </c>
+      <c r="I51">
+        <v>2</v>
+      </c>
+      <c r="J51">
+        <v>25</v>
+      </c>
+      <c r="K51" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+      <c r="D52" t="s">
+        <v>85</v>
+      </c>
+      <c r="E52">
+        <v>5</v>
+      </c>
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="G52">
+        <v>25</v>
+      </c>
+      <c r="I52">
+        <v>4</v>
+      </c>
+      <c r="J52">
+        <v>25</v>
+      </c>
+      <c r="K52" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>51</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>3</v>
+      </c>
+      <c r="D53" t="s">
+        <v>86</v>
+      </c>
+      <c r="E53">
+        <v>5</v>
+      </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+      <c r="G53">
+        <v>25</v>
+      </c>
+      <c r="I53">
+        <v>6</v>
+      </c>
+      <c r="J53">
+        <v>25</v>
+      </c>
+      <c r="K53" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>52</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>3</v>
+      </c>
+      <c r="D54" t="s">
+        <v>84</v>
+      </c>
+      <c r="E54">
+        <v>6</v>
+      </c>
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="G54">
+        <v>26</v>
+      </c>
+      <c r="I54">
+        <v>2</v>
+      </c>
+      <c r="J54">
+        <v>26</v>
+      </c>
+      <c r="K54" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>53</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>3</v>
+      </c>
+      <c r="D55" t="s">
+        <v>85</v>
+      </c>
+      <c r="E55">
+        <v>6</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55">
+        <v>26</v>
+      </c>
+      <c r="I55">
+        <v>4</v>
+      </c>
+      <c r="J55">
+        <v>26</v>
+      </c>
+      <c r="K55" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>3</v>
+      </c>
+      <c r="D56" t="s">
+        <v>86</v>
+      </c>
+      <c r="E56">
+        <v>6</v>
+      </c>
+      <c r="F56">
+        <v>1</v>
+      </c>
+      <c r="G56">
+        <v>26</v>
+      </c>
+      <c r="I56">
+        <v>6</v>
+      </c>
+      <c r="J56">
+        <v>26</v>
+      </c>
+      <c r="K56" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>55</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>3</v>
+      </c>
+      <c r="D57" t="s">
+        <v>84</v>
+      </c>
+      <c r="E57">
+        <v>7</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="G57">
+        <v>27</v>
+      </c>
+      <c r="I57">
+        <v>2</v>
+      </c>
+      <c r="J57">
+        <v>27</v>
+      </c>
+      <c r="K57" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>56</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>3</v>
+      </c>
+      <c r="D58" t="s">
+        <v>85</v>
+      </c>
+      <c r="E58">
+        <v>7</v>
+      </c>
+      <c r="F58">
+        <v>1</v>
+      </c>
+      <c r="G58">
+        <v>27</v>
+      </c>
+      <c r="I58">
+        <v>4</v>
+      </c>
+      <c r="J58">
+        <v>27</v>
+      </c>
+      <c r="K58" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>57</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59">
+        <v>3</v>
+      </c>
+      <c r="D59" t="s">
+        <v>86</v>
+      </c>
+      <c r="E59">
+        <v>7</v>
+      </c>
+      <c r="F59">
+        <v>1</v>
+      </c>
+      <c r="G59">
+        <v>27</v>
+      </c>
+      <c r="I59">
+        <v>6</v>
+      </c>
+      <c r="J59">
+        <v>27</v>
+      </c>
+      <c r="K59" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>58</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60">
+        <v>3</v>
+      </c>
+      <c r="D60" t="s">
+        <v>84</v>
+      </c>
+      <c r="E60">
+        <v>8</v>
+      </c>
+      <c r="F60">
+        <v>1</v>
+      </c>
+      <c r="G60">
+        <v>28</v>
+      </c>
+      <c r="I60">
+        <v>2</v>
+      </c>
+      <c r="J60">
+        <v>28</v>
+      </c>
+      <c r="K60" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>59</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61">
+        <v>3</v>
+      </c>
+      <c r="D61" t="s">
+        <v>85</v>
+      </c>
+      <c r="E61">
+        <v>8</v>
+      </c>
+      <c r="F61">
+        <v>1</v>
+      </c>
+      <c r="G61">
+        <v>28</v>
+      </c>
+      <c r="I61">
+        <v>4</v>
+      </c>
+      <c r="J61">
+        <v>28</v>
+      </c>
+      <c r="K61" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>60</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>3</v>
+      </c>
+      <c r="D62" t="s">
+        <v>86</v>
+      </c>
+      <c r="E62">
+        <v>8</v>
+      </c>
+      <c r="F62">
+        <v>1</v>
+      </c>
+      <c r="G62">
+        <v>28</v>
+      </c>
+      <c r="I62">
+        <v>6</v>
+      </c>
+      <c r="J62">
+        <v>28</v>
+      </c>
+      <c r="K62" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>61</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <v>3</v>
+      </c>
+      <c r="D63" t="s">
+        <v>84</v>
+      </c>
+      <c r="E63">
+        <v>9</v>
+      </c>
+      <c r="F63">
+        <v>1</v>
+      </c>
+      <c r="G63">
+        <v>29</v>
+      </c>
+      <c r="I63">
+        <v>2</v>
+      </c>
+      <c r="J63">
+        <v>29</v>
+      </c>
+      <c r="K63" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>62</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64">
+        <v>3</v>
+      </c>
+      <c r="D64" t="s">
+        <v>85</v>
+      </c>
+      <c r="E64">
+        <v>9</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
+      </c>
+      <c r="G64">
+        <v>29</v>
+      </c>
+      <c r="I64">
+        <v>4</v>
+      </c>
+      <c r="J64">
+        <v>29</v>
+      </c>
+      <c r="K64" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>63</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="C65">
+        <v>3</v>
+      </c>
+      <c r="D65" t="s">
+        <v>86</v>
+      </c>
+      <c r="E65">
+        <v>9</v>
+      </c>
+      <c r="F65">
+        <v>1</v>
+      </c>
+      <c r="G65">
+        <v>29</v>
+      </c>
+      <c r="I65">
+        <v>6</v>
+      </c>
+      <c r="J65">
+        <v>29</v>
+      </c>
+      <c r="K65" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>64</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66">
+        <v>3</v>
+      </c>
+      <c r="D66" t="s">
+        <v>84</v>
+      </c>
+      <c r="E66">
+        <v>10</v>
+      </c>
+      <c r="F66">
+        <v>1</v>
+      </c>
+      <c r="G66">
+        <v>30</v>
+      </c>
+      <c r="I66">
+        <v>2</v>
+      </c>
+      <c r="J66">
+        <v>30</v>
+      </c>
+      <c r="K66" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>65</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67">
+        <v>3</v>
+      </c>
+      <c r="D67" t="s">
+        <v>85</v>
+      </c>
+      <c r="E67">
+        <v>10</v>
+      </c>
+      <c r="F67">
+        <v>1</v>
+      </c>
+      <c r="G67">
+        <v>30</v>
+      </c>
+      <c r="I67">
+        <v>4</v>
+      </c>
+      <c r="J67">
+        <v>30</v>
+      </c>
+      <c r="K67" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>66</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68">
+        <v>3</v>
+      </c>
+      <c r="D68" t="s">
+        <v>86</v>
+      </c>
+      <c r="E68">
+        <v>10</v>
+      </c>
+      <c r="F68">
+        <v>1</v>
+      </c>
+      <c r="G68">
+        <v>30</v>
+      </c>
+      <c r="I68">
+        <v>6</v>
+      </c>
+      <c r="J68">
+        <v>30</v>
+      </c>
+      <c r="K68" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>67</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69">
+        <v>3</v>
+      </c>
+      <c r="D69" t="s">
+        <v>84</v>
+      </c>
+      <c r="E69">
+        <v>11</v>
+      </c>
+      <c r="F69">
+        <v>1</v>
+      </c>
+      <c r="G69">
+        <v>31</v>
+      </c>
+      <c r="I69">
+        <v>2</v>
+      </c>
+      <c r="J69">
+        <v>31</v>
+      </c>
+      <c r="K69" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>68</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70">
+        <v>3</v>
+      </c>
+      <c r="D70" t="s">
+        <v>85</v>
+      </c>
+      <c r="E70">
+        <v>11</v>
+      </c>
+      <c r="F70">
+        <v>1</v>
+      </c>
+      <c r="G70">
+        <v>31</v>
+      </c>
+      <c r="I70">
+        <v>4</v>
+      </c>
+      <c r="J70">
+        <v>31</v>
+      </c>
+      <c r="K70" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>69</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="C71">
+        <v>3</v>
+      </c>
+      <c r="D71" t="s">
+        <v>86</v>
+      </c>
+      <c r="E71">
+        <v>11</v>
+      </c>
+      <c r="F71">
+        <v>1</v>
+      </c>
+      <c r="G71">
+        <v>31</v>
+      </c>
+      <c r="I71">
+        <v>6</v>
+      </c>
+      <c r="J71">
+        <v>31</v>
+      </c>
+      <c r="K71" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>70</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="C72">
+        <v>3</v>
+      </c>
+      <c r="D72" t="s">
+        <v>84</v>
+      </c>
+      <c r="E72">
+        <v>12</v>
+      </c>
+      <c r="F72">
+        <v>1</v>
+      </c>
+      <c r="G72">
+        <v>32</v>
+      </c>
+      <c r="I72">
+        <v>2</v>
+      </c>
+      <c r="J72">
+        <v>32</v>
+      </c>
+      <c r="K72" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>71</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73">
+        <v>3</v>
+      </c>
+      <c r="D73" t="s">
+        <v>85</v>
+      </c>
+      <c r="E73">
+        <v>12</v>
+      </c>
+      <c r="F73">
+        <v>1</v>
+      </c>
+      <c r="G73">
+        <v>32</v>
+      </c>
+      <c r="I73">
+        <v>4</v>
+      </c>
+      <c r="J73">
+        <v>32</v>
+      </c>
+      <c r="K73" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>72</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B74">
+        <v>1</v>
+      </c>
+      <c r="C74">
+        <v>3</v>
+      </c>
+      <c r="D74" t="s">
+        <v>86</v>
+      </c>
+      <c r="E74">
+        <v>12</v>
+      </c>
+      <c r="F74">
+        <v>1</v>
+      </c>
+      <c r="G74">
+        <v>32</v>
+      </c>
+      <c r="I74">
+        <v>6</v>
+      </c>
+      <c r="J74">
+        <v>32</v>
+      </c>
+      <c r="K74" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>73</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B75">
+        <v>1</v>
+      </c>
+      <c r="C75">
+        <v>3</v>
+      </c>
+      <c r="D75" t="s">
+        <v>84</v>
+      </c>
+      <c r="E75">
+        <v>13</v>
+      </c>
+      <c r="F75">
+        <v>1</v>
+      </c>
+      <c r="G75">
+        <v>33</v>
+      </c>
+      <c r="I75">
+        <v>2</v>
+      </c>
+      <c r="J75">
+        <v>33</v>
+      </c>
+      <c r="K75" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>74</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B76">
+        <v>1</v>
+      </c>
+      <c r="C76">
+        <v>3</v>
+      </c>
+      <c r="D76" t="s">
+        <v>85</v>
+      </c>
+      <c r="E76">
+        <v>13</v>
+      </c>
+      <c r="F76">
+        <v>1</v>
+      </c>
+      <c r="G76">
+        <v>33</v>
+      </c>
+      <c r="I76">
+        <v>4</v>
+      </c>
+      <c r="J76">
+        <v>33</v>
+      </c>
+      <c r="K76" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>75</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77">
+        <v>3</v>
+      </c>
+      <c r="D77" t="s">
+        <v>86</v>
+      </c>
+      <c r="E77">
+        <v>13</v>
+      </c>
+      <c r="F77">
+        <v>1</v>
+      </c>
+      <c r="G77">
+        <v>33</v>
+      </c>
+      <c r="I77">
+        <v>6</v>
+      </c>
+      <c r="J77">
+        <v>33</v>
+      </c>
+      <c r="K77" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>76</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B78">
+        <v>1</v>
+      </c>
+      <c r="C78">
+        <v>3</v>
+      </c>
+      <c r="D78" t="s">
+        <v>84</v>
+      </c>
+      <c r="E78">
+        <v>14</v>
+      </c>
+      <c r="F78">
+        <v>1</v>
+      </c>
+      <c r="G78">
+        <v>34</v>
+      </c>
+      <c r="I78">
+        <v>2</v>
+      </c>
+      <c r="J78">
+        <v>34</v>
+      </c>
+      <c r="K78" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>77</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B79">
+        <v>1</v>
+      </c>
+      <c r="C79">
+        <v>3</v>
+      </c>
+      <c r="D79" t="s">
+        <v>85</v>
+      </c>
+      <c r="E79">
+        <v>14</v>
+      </c>
+      <c r="F79">
+        <v>1</v>
+      </c>
+      <c r="G79">
+        <v>34</v>
+      </c>
+      <c r="I79">
+        <v>4</v>
+      </c>
+      <c r="J79">
+        <v>34</v>
+      </c>
+      <c r="K79" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>78</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B80">
+        <v>1</v>
+      </c>
+      <c r="C80">
+        <v>3</v>
+      </c>
+      <c r="D80" t="s">
+        <v>86</v>
+      </c>
+      <c r="E80">
+        <v>14</v>
+      </c>
+      <c r="F80">
+        <v>1</v>
+      </c>
+      <c r="G80">
+        <v>34</v>
+      </c>
+      <c r="I80">
+        <v>6</v>
+      </c>
+      <c r="J80">
+        <v>34</v>
+      </c>
+      <c r="K80" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>79</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B81">
+        <v>1</v>
+      </c>
+      <c r="C81">
+        <v>3</v>
+      </c>
+      <c r="D81" t="s">
+        <v>84</v>
+      </c>
+      <c r="E81">
+        <v>15</v>
+      </c>
+      <c r="F81">
+        <v>1</v>
+      </c>
+      <c r="G81">
+        <v>35</v>
+      </c>
+      <c r="I81">
+        <v>2</v>
+      </c>
+      <c r="J81">
+        <v>35</v>
+      </c>
+      <c r="K81" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>80</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B82">
+        <v>1</v>
+      </c>
+      <c r="C82">
+        <v>3</v>
+      </c>
+      <c r="D82" t="s">
+        <v>85</v>
+      </c>
+      <c r="E82">
+        <v>15</v>
+      </c>
+      <c r="F82">
+        <v>1</v>
+      </c>
+      <c r="G82">
+        <v>35</v>
+      </c>
+      <c r="I82">
+        <v>4</v>
+      </c>
+      <c r="J82">
+        <v>35</v>
+      </c>
+      <c r="K82" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>81</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B83">
+        <v>1</v>
+      </c>
+      <c r="C83">
+        <v>3</v>
+      </c>
+      <c r="D83" t="s">
+        <v>86</v>
+      </c>
+      <c r="E83">
+        <v>15</v>
+      </c>
+      <c r="F83">
+        <v>1</v>
+      </c>
+      <c r="G83">
+        <v>35</v>
+      </c>
+      <c r="I83">
+        <v>6</v>
+      </c>
+      <c r="J83">
+        <v>35</v>
+      </c>
+      <c r="K83" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>82</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B84">
+        <v>1</v>
+      </c>
+      <c r="C84">
+        <v>3</v>
+      </c>
+      <c r="D84" t="s">
+        <v>84</v>
+      </c>
+      <c r="E84">
+        <v>16</v>
+      </c>
+      <c r="F84">
+        <v>1</v>
+      </c>
+      <c r="G84">
+        <v>36</v>
+      </c>
+      <c r="I84">
+        <v>2</v>
+      </c>
+      <c r="J84">
+        <v>36</v>
+      </c>
+      <c r="K84" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>83</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B85">
+        <v>1</v>
+      </c>
+      <c r="C85">
+        <v>3</v>
+      </c>
+      <c r="D85" t="s">
+        <v>85</v>
+      </c>
+      <c r="E85">
+        <v>16</v>
+      </c>
+      <c r="F85">
+        <v>1</v>
+      </c>
+      <c r="G85">
+        <v>36</v>
+      </c>
+      <c r="I85">
+        <v>4</v>
+      </c>
+      <c r="J85">
+        <v>36</v>
+      </c>
+      <c r="K85" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>84</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B86">
+        <v>1</v>
+      </c>
+      <c r="C86">
+        <v>3</v>
+      </c>
+      <c r="D86" t="s">
+        <v>86</v>
+      </c>
+      <c r="E86">
+        <v>16</v>
+      </c>
+      <c r="F86">
+        <v>1</v>
+      </c>
+      <c r="G86">
+        <v>36</v>
+      </c>
+      <c r="I86">
+        <v>6</v>
+      </c>
+      <c r="J86">
+        <v>36</v>
+      </c>
+      <c r="K86" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>85</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B87">
+        <v>1</v>
+      </c>
+      <c r="C87">
+        <v>3</v>
+      </c>
+      <c r="D87" t="s">
+        <v>84</v>
+      </c>
+      <c r="E87">
+        <v>17</v>
+      </c>
+      <c r="F87">
+        <v>1</v>
+      </c>
+      <c r="G87">
+        <v>37</v>
+      </c>
+      <c r="I87">
+        <v>2</v>
+      </c>
+      <c r="J87">
+        <v>37</v>
+      </c>
+      <c r="K87" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>86</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B88">
+        <v>1</v>
+      </c>
+      <c r="C88">
+        <v>3</v>
+      </c>
+      <c r="D88" t="s">
+        <v>85</v>
+      </c>
+      <c r="E88">
+        <v>17</v>
+      </c>
+      <c r="F88">
+        <v>1</v>
+      </c>
+      <c r="G88">
+        <v>37</v>
+      </c>
+      <c r="I88">
+        <v>4</v>
+      </c>
+      <c r="J88">
+        <v>37</v>
+      </c>
+      <c r="K88" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>87</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B89">
+        <v>1</v>
+      </c>
+      <c r="C89">
+        <v>3</v>
+      </c>
+      <c r="D89" t="s">
+        <v>86</v>
+      </c>
+      <c r="E89">
+        <v>17</v>
+      </c>
+      <c r="F89">
+        <v>1</v>
+      </c>
+      <c r="G89">
+        <v>37</v>
+      </c>
+      <c r="I89">
+        <v>6</v>
+      </c>
+      <c r="J89">
+        <v>37</v>
+      </c>
+      <c r="K89" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>88</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B90">
+        <v>1</v>
+      </c>
+      <c r="C90">
+        <v>3</v>
+      </c>
+      <c r="D90" t="s">
+        <v>87</v>
+      </c>
+      <c r="E90" t="s">
+        <v>87</v>
+      </c>
+      <c r="F90">
+        <v>1</v>
+      </c>
+      <c r="G90">
+        <v>37</v>
+      </c>
+      <c r="I90">
+        <v>4</v>
+      </c>
+      <c r="J90">
+        <v>39</v>
+      </c>
+      <c r="K90" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>89</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B91">
+        <v>1</v>
+      </c>
+      <c r="C91">
+        <v>3</v>
+      </c>
+      <c r="D91" t="s">
+        <v>88</v>
+      </c>
+      <c r="E91" t="s">
+        <v>91</v>
+      </c>
+      <c r="F91">
+        <v>4</v>
+      </c>
+      <c r="G91">
+        <v>42</v>
+      </c>
+      <c r="I91">
+        <v>4</v>
+      </c>
+      <c r="J91">
+        <v>43</v>
+      </c>
+      <c r="K91" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>90</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B92">
+        <v>1</v>
+      </c>
+      <c r="C92">
+        <v>3</v>
+      </c>
+      <c r="D92" t="s">
+        <v>89</v>
+      </c>
+      <c r="E92" t="s">
+        <v>73</v>
+      </c>
+      <c r="F92">
+        <v>5</v>
+      </c>
+      <c r="G92">
+        <v>42</v>
+      </c>
+      <c r="I92">
+        <v>5</v>
+      </c>
+      <c r="J92">
+        <v>43</v>
+      </c>
+      <c r="K92" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>91</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B93">
+        <v>1</v>
+      </c>
+      <c r="C93">
+        <v>3</v>
+      </c>
+      <c r="D93" t="s">
+        <v>90</v>
+      </c>
+      <c r="E93" t="s">
+        <v>79</v>
+      </c>
+      <c r="F93">
+        <v>7</v>
+      </c>
+      <c r="G93">
+        <v>42</v>
+      </c>
+      <c r="I93">
+        <v>7</v>
+      </c>
+      <c r="J93">
+        <v>43</v>
+      </c>
+      <c r="K93" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>94</v>
       </c>

</xml_diff>